<commit_message>
fisrt commit before change to period list
</commit_message>
<xml_diff>
--- a/data/t2m_classification.xlsx
+++ b/data/t2m_classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\t2m-project\t2m-pycode\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A6E90-AB53-4E31-A403-35AE3B172444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3EE583-40E3-4063-9C9A-489458A3EC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_stock_list" sheetId="1" r:id="rId1"/>
@@ -6378,7 +6378,7 @@
   <dimension ref="A1:H516"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>